<commit_message>
2021 Excess Mortality Update
</commit_message>
<xml_diff>
--- a/myCCB/www/xMDA/xMDA_tables/figure-1-table.xlsx
+++ b/myCCB/www/xMDA/xMDA_tables/figure-1-table.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Year-Quarter</t>
   </si>
@@ -69,12 +69,21 @@
   </si>
   <si>
     <t xml:space="preserve">2021 Q1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 Q3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021 Q4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -114,8 +123,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:B18" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:B18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:B21" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:B21"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Year-Quarter"/>
     <tableColumn id="2" name="All-Cause Age-Adjusted Death Rate"/>
@@ -402,10 +411,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -546,7 +555,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="n">
-        <v>193.8</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18">
@@ -554,7 +563,31 @@
         <v>18</v>
       </c>
       <c r="B18" t="n">
-        <v>213.9</v>
+        <v>214.5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="n">
+        <v>142.7</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="n">
+        <v>160.7</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="n">
+        <v>167.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>